<commit_message>
Fix IC1/3 thing in BOM
</commit_message>
<xml_diff>
--- a/m50,m40,m60 Pnp/Rev 2.2/BOM-speeduino v0.4.3 compatible PCB for m50nv rev2.2.xlsx
+++ b/m50,m40,m60 Pnp/Rev 2.2/BOM-speeduino v0.4.3 compatible PCB for m50nv rev2.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m50,m40,m60 Pnp\Rev 2.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D37AA32-7BD0-40D0-85DE-53FC955D18FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BF0753-19A3-4338-9A38-C45EC09770A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="495" yWindow="735" windowWidth="28650" windowHeight="14850" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="30" windowWidth="27975" windowHeight="15570" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -1249,10 +1249,10 @@
     </r>
   </si>
   <si>
-    <t>IC1,IC2,IC5</t>
-  </si>
-  <si>
     <t>C1,C3,C5,C7,C9,C13,C15,C21,C22,C29</t>
+  </si>
+  <si>
+    <t>IC2,IC3,IC5</t>
   </si>
 </sst>
 </file>
@@ -2041,8 +2041,8 @@
   </sheetPr>
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2268,7 +2268,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>13</v>
@@ -4463,7 +4463,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>94</v>

</xml_diff>